<commit_message>
makemuzicodes tool support code action; default action; fix some bugs
</commit_message>
<xml_diff>
--- a/scoretools/test/test1.xlsx
+++ b/scoretools/test/test1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
   <si>
     <t>stage</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>basecamp.jpg</t>
+  </si>
+  <si>
+    <t>2b</t>
   </si>
 </sst>
 </file>
@@ -446,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,6 +635,9 @@
       <c r="G4" t="s">
         <v>10</v>
       </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -654,6 +660,11 @@
       </c>
       <c r="G5" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add weather to makemuzicodes
</commit_message>
<xml_diff>
--- a/scoretools/test/test1.xlsx
+++ b/scoretools/test/test1.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pszcmg\workspace\fast-performance-demo\scoretools\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28380" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
   <si>
     <t>stage</t>
   </si>
@@ -123,6 +121,15 @@
   </si>
   <si>
     <t>2b</t>
+  </si>
+  <si>
+    <t>midi</t>
+  </si>
+  <si>
+    <t>903a7f</t>
+  </si>
+  <si>
+    <t>no_effect</t>
   </si>
 </sst>
 </file>
@@ -229,7 +236,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,7 +271,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -441,7 +448,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -449,18 +456,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="17" width="12.140625" customWidth="1"/>
+    <col min="1" max="19" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,73 +475,79 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -542,7 +555,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -557,31 +570,37 @@
         <v>3</v>
       </c>
       <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>31</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>13</v>
       </c>
-      <c r="R2" t="s">
+      <c r="Q2" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" t="s">
         <v>14</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>4</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>15</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -589,11 +608,11 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
@@ -601,19 +620,22 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>11</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>16</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -621,25 +643,28 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
       <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
-        <v>3</v>
-      </c>
       <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
         <v>10</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -661,14 +686,22 @@
       <c r="G5" t="s">
         <v>3</v>
       </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26">
       <c r="A6" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added initial images and contenturi config
</commit_message>
<xml_diff>
--- a/scoretools/test/test1.xlsx
+++ b/scoretools/test/test1.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pszcmg\workspace\fast-performance-demo\scoretools\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
   <si>
     <t>stage</t>
   </si>
@@ -117,9 +122,6 @@
     <t>mc3:</t>
   </si>
   <si>
-    <t>basecamp.jpg</t>
-  </si>
-  <si>
     <t>2b</t>
   </si>
   <si>
@@ -130,6 +132,12 @@
   </si>
   <si>
     <t>no_effect</t>
+  </si>
+  <si>
+    <t>baseCamp.jpg</t>
+  </si>
+  <si>
+    <t>ending.jpg</t>
   </si>
 </sst>
 </file>
@@ -448,7 +456,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -456,18 +464,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z6"/>
+  <dimension ref="A1:AB6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="19" width="12.1640625" customWidth="1"/>
+    <col min="1" max="21" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +483,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>17</v>
@@ -502,52 +510,58 @@
         <v>24</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="R1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -575,32 +589,35 @@
       <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>5</v>
       </c>
-      <c r="M2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="N2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" t="s">
-        <v>34</v>
+      <c r="R2" t="s">
+        <v>33</v>
       </c>
       <c r="T2" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" t="s">
         <v>14</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>4</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>15</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -628,14 +645,14 @@
       <c r="I3" t="s">
         <v>11</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>16</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -661,10 +678,10 @@
         <v>10</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -690,9 +707,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added readmei and meiutils; read in makemusicodes
</commit_message>
<xml_diff>
--- a/scoretools/test/test1.xlsx
+++ b/scoretools/test/test1.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pszcmg\workspace\fast-performance-demo\scoretools\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15525"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
   <si>
     <t>stage</t>
   </si>
@@ -47,9 +42,6 @@
     <t>data:text/plain,Base Camp</t>
   </si>
   <si>
-    <t>bc.mei</t>
-  </si>
-  <si>
     <t>1b.mei</t>
   </si>
   <si>
@@ -138,6 +130,18 @@
   </si>
   <si>
     <t>ending.jpg</t>
+  </si>
+  <si>
+    <t>MSThe Climb (Base Camp).mei</t>
+  </si>
+  <si>
+    <t>Ending 2</t>
+  </si>
+  <si>
+    <t>Ending 1</t>
+  </si>
+  <si>
+    <t>Ending 3</t>
   </si>
 </sst>
 </file>
@@ -456,7 +460,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -466,16 +470,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="21" width="12.140625" customWidth="1"/>
+    <col min="1" max="21" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,93 +487,93 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -593,123 +597,132 @@
         <v>5</v>
       </c>
       <c r="N2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" t="s">
         <v>35</v>
       </c>
-      <c r="P2" t="s">
+      <c r="U2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" t="s">
         <v>13</v>
-      </c>
-      <c r="R2" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" t="s">
-        <v>14</v>
       </c>
       <c r="W2" t="s">
         <v>4</v>
       </c>
+      <c r="Y2" t="s">
+        <v>39</v>
+      </c>
       <c r="Z2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:28">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="P3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>8</v>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>